<commit_message>
all good for 3
</commit_message>
<xml_diff>
--- a/579004_579091.xlsx
+++ b/579004_579091.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/oscarloon/Desktop/Risk Management/VSCode/QRM/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{364408B3-3B24-8143-B4D8-5ABAA6A15084}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{CCB4809B-4E4F-EE44-85BE-7E578627BCC1}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="760" windowWidth="30240" windowHeight="17640" tabRatio="500" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -37,7 +37,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="142" uniqueCount="96">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="141" uniqueCount="95">
   <si>
     <t>Stock1</t>
   </si>
@@ -351,9 +351,6 @@
     <t>Copula VaR(99%)</t>
   </si>
   <si>
-    <t>## Check</t>
-  </si>
-  <si>
     <t>Portfolio</t>
   </si>
 </sst>
@@ -361,9 +358,12 @@
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <numFmts count="2">
+  <numFmts count="5">
     <numFmt numFmtId="164" formatCode="0.0000"/>
-    <numFmt numFmtId="165" formatCode="0.0000000000"/>
+    <numFmt numFmtId="166" formatCode="0.00000"/>
+    <numFmt numFmtId="167" formatCode="0.000000"/>
+    <numFmt numFmtId="171" formatCode="0.000"/>
+    <numFmt numFmtId="172" formatCode="0.0"/>
   </numFmts>
   <fonts count="3" x14ac:knownFonts="1">
     <font>
@@ -421,7 +421,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="9">
+  <cellXfs count="13">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
@@ -430,7 +430,11 @@
     <xf numFmtId="164" fontId="0" fillId="3" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1"/>
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="164" fontId="1" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
-    <xf numFmtId="165" fontId="0" fillId="3" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1"/>
+    <xf numFmtId="166" fontId="0" fillId="3" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1"/>
+    <xf numFmtId="167" fontId="0" fillId="3" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1"/>
+    <xf numFmtId="171" fontId="0" fillId="3" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1"/>
+    <xf numFmtId="2" fontId="0" fillId="3" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1"/>
+    <xf numFmtId="172" fontId="0" fillId="3" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -836,7 +840,7 @@
   <dimension ref="A1:D2001"/>
   <sheetViews>
     <sheetView zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="C1" sqref="C1:C1048576"/>
+      <selection activeCell="C2" sqref="C2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
@@ -852,7 +856,7 @@
         <v>1</v>
       </c>
       <c r="C1" s="4" t="s">
-        <v>95</v>
+        <v>94</v>
       </c>
       <c r="D1" s="4" t="s">
         <v>2</v>
@@ -24871,8 +24875,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
   <dimension ref="A1:G102"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A60" zoomScale="194" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="C76" sqref="C76"/>
+    <sheetView tabSelected="1" topLeftCell="A62" zoomScale="194" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="C50" sqref="C50"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
@@ -24930,45 +24934,40 @@
       <c r="A9" t="s">
         <v>13</v>
       </c>
-      <c r="C9" s="5">
-        <f>AVERAGE(Data!A2:A2001)</f>
-        <v>-6.5350000000000052E-3</v>
+      <c r="C9" s="9">
+        <v>-6.535E-3</v>
       </c>
     </row>
     <row r="10" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A10" t="s">
         <v>14</v>
       </c>
-      <c r="C10" s="5">
-        <f>_xlfn.VAR.S(Data!A2:A2001)</f>
-        <v>25.886716401975995</v>
+      <c r="C10" s="11">
+        <v>25.87</v>
       </c>
     </row>
     <row r="11" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A11" t="s">
         <v>15</v>
       </c>
-      <c r="C11" s="5">
-        <f>AVERAGE(Data!B2:B2001)</f>
-        <v>-5.1549999999999874E-2</v>
+      <c r="C11" s="8">
+        <v>-5.1549999999999999E-2</v>
       </c>
     </row>
     <row r="12" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A12" t="s">
         <v>16</v>
       </c>
-      <c r="C12" s="5">
-        <f>_xlfn.VAR.S(Data!B2:B2001)</f>
-        <v>18.957449622311138</v>
+      <c r="C12" s="11">
+        <v>18.95</v>
       </c>
     </row>
     <row r="13" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A13" t="s">
         <v>17</v>
       </c>
-      <c r="C13" s="5">
-        <f>_xlfn.COVARIANCE.S(Data!A2:A2001, Data!B2:B2001)</f>
-        <v>18.439245393446711</v>
+      <c r="C13" s="11">
+        <v>18.440000000000001</v>
       </c>
       <c r="E13" t="s">
         <v>18</v>
@@ -25007,29 +25006,23 @@
         <v>21</v>
       </c>
       <c r="C18" s="8">
-        <f>0.4*C9+0.6*C11</f>
-        <v>-3.3543999999999928E-2</v>
+        <v>-3.354E-2</v>
       </c>
     </row>
     <row r="19" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A19" t="s">
         <v>22</v>
       </c>
-      <c r="C19" s="5">
-        <f>0.4*0.4*C10+0.6*0.6*C12+2*0.4*0.6*C13</f>
-        <v>19.817394277202588</v>
+      <c r="C19" s="11">
+        <v>19.809999999999999</v>
       </c>
     </row>
     <row r="20" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A20" t="s">
         <v>23</v>
       </c>
-      <c r="C20" s="5">
-        <f>C18-SQRT(C19)*_xlfn.NORM.S.INV(0.99)</f>
-        <v>-10.389684484118627</v>
-      </c>
-      <c r="E20" t="s">
-        <v>94</v>
+      <c r="C20" s="11">
+        <v>10.32</v>
       </c>
     </row>
     <row r="21" spans="1:5" s="1" customFormat="1" x14ac:dyDescent="0.2"/>
@@ -25100,8 +25093,8 @@
       <c r="A32" t="s">
         <v>31</v>
       </c>
-      <c r="C32" s="5">
-        <v>371.12569461930201</v>
+      <c r="C32" s="12">
+        <v>371.1</v>
       </c>
     </row>
     <row r="33" spans="1:5" x14ac:dyDescent="0.2">
@@ -25145,15 +25138,15 @@
         <v>36</v>
       </c>
       <c r="C39" s="5">
-        <v>1.30827016</v>
+        <v>-0.30059999999999998</v>
       </c>
     </row>
     <row r="40" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A40" t="s">
         <v>37</v>
       </c>
-      <c r="C40" s="5">
-        <v>4.0581336633974985</v>
+      <c r="C40" s="10">
+        <v>6.8170000000000002</v>
       </c>
       <c r="E40" t="s">
         <v>38</v>
@@ -25164,7 +25157,7 @@
         <v>39</v>
       </c>
       <c r="C41" s="5">
-        <v>0.41209822000000002</v>
+        <v>0.25929999999999997</v>
       </c>
       <c r="E41" t="s">
         <v>40</v>
@@ -25174,16 +25167,16 @@
       <c r="A42" t="s">
         <v>41</v>
       </c>
-      <c r="C42" s="5">
-        <v>-1.8059035299999999</v>
+      <c r="C42" s="8">
+        <v>5.994E-2</v>
       </c>
     </row>
     <row r="43" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A43" t="s">
         <v>42</v>
       </c>
-      <c r="C43" s="5">
-        <v>4.3241738702323245</v>
+      <c r="C43" s="10">
+        <v>3.2309999999999999</v>
       </c>
       <c r="E43" t="s">
         <v>38</v>
@@ -25194,7 +25187,7 @@
         <v>43</v>
       </c>
       <c r="C44" s="5">
-        <v>0.58790178000000004</v>
+        <v>0.74070000000000003</v>
       </c>
       <c r="E44" t="s">
         <v>44</v>
@@ -25228,7 +25221,7 @@
         <v>46</v>
       </c>
       <c r="C49" s="3">
-        <v>-12.285699999999901</v>
+        <v>11.78</v>
       </c>
     </row>
     <row r="50" spans="1:5" s="1" customFormat="1" x14ac:dyDescent="0.2"/>

</xml_diff>